<commit_message>
Add some 3D print model.
还编造了方案说明
</commit_message>
<xml_diff>
--- a/doc/BOM.xlsx
+++ b/doc/BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C4E42EA9-12CB-4FAB-BBE7-0D3B3778986F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BE32F6E3-9939-4424-9938-B21C85CD67CD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="75">
   <si>
     <t>项目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -181,14 +181,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4s5300mah 30c</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最好多买两块，品牌待定</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>总重</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -266,6 +258,62 @@
   </si>
   <si>
     <t>需要评估重量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>减重减配方案</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>没救</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>换成9g舵机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可能还会增重</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以换成6303或者副厂</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>乐迪Mini Pix有望轻几克</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不装</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>把电池里的铝板拆了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>格氏4s5300mah 30c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最好多买两块</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自己拿kt板削</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设计高端结构</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大概可以铣薄减重？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开减重孔</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -430,6 +478,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-F6F4-49E0-9687-0DED38437BB9}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -445,6 +498,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-F6F4-49E0-9687-0DED38437BB9}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -460,6 +518,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-F6F4-49E0-9687-0DED38437BB9}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -475,6 +538,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-F6F4-49E0-9687-0DED38437BB9}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -490,6 +558,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-F6F4-49E0-9687-0DED38437BB9}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -527,7 +600,7 @@
                   <c:v>505</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1065</c:v>
+                  <c:v>1230</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>437</c:v>
@@ -729,6 +802,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-1F9E-4EF9-9DD8-DB63BC14735D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -744,6 +822,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-1F9E-4EF9-9DD8-DB63BC14735D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -759,6 +842,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-1F9E-4EF9-9DD8-DB63BC14735D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -774,6 +862,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-1F9E-4EF9-9DD8-DB63BC14735D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -789,6 +882,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-1F9E-4EF9-9DD8-DB63BC14735D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -2059,16 +2157,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1385887</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>185737</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2095,16 +2193,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1385887</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>814388</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>185737</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>885826</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2453,10 +2551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2465,12 +2563,13 @@
     <col min="2" max="2" width="29.5" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
     <col min="4" max="5" width="9" customWidth="1"/>
-    <col min="9" max="9" width="41" customWidth="1"/>
-    <col min="10" max="10" width="19.75" customWidth="1"/>
-    <col min="14" max="14" width="29" customWidth="1"/>
+    <col min="9" max="9" width="21.875" customWidth="1"/>
+    <col min="10" max="10" width="41" customWidth="1"/>
+    <col min="11" max="11" width="19.75" customWidth="1"/>
+    <col min="15" max="15" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2484,7 +2583,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -2496,10 +2595,13 @@
         <v>36</v>
       </c>
       <c r="I1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2526,11 +2628,14 @@
         <f>G2*1.1</f>
         <v>1317.8000000000002</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>59</v>
+      <c r="I2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2551,15 +2656,18 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <f>F3*D3</f>
+        <f t="shared" ref="G3:G18" si="1">F3*D3</f>
         <v>0</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H18" si="1">G3*1.1</f>
+        <f t="shared" ref="H3:H18" si="2">G3*1.1</f>
         <v>0</v>
       </c>
+      <c r="I3" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2580,15 +2688,18 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <f>F4*D4</f>
-        <v>0</v>
-      </c>
-      <c r="H4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="H4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2609,18 +2720,21 @@
         <v>35</v>
       </c>
       <c r="G5">
-        <f>F5*D5</f>
+        <f t="shared" si="1"/>
         <v>245</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>269.5</v>
       </c>
       <c r="I5" t="s">
-        <v>44</v>
+        <v>63</v>
+      </c>
+      <c r="J5" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -2641,18 +2755,21 @@
         <v>300</v>
       </c>
       <c r="G6">
-        <f>F6*D6</f>
+        <f t="shared" si="1"/>
         <v>600</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>660</v>
       </c>
       <c r="I6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2673,15 +2790,18 @@
         <v>760</v>
       </c>
       <c r="G7">
-        <f>F7*D7</f>
+        <f t="shared" si="1"/>
         <v>760</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>836.00000000000011</v>
       </c>
+      <c r="I7" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2702,15 +2822,18 @@
         <v>1422</v>
       </c>
       <c r="G8">
-        <f>F8*D8</f>
+        <f t="shared" si="1"/>
         <v>1422</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1564.2</v>
       </c>
+      <c r="I8" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2731,23 +2854,26 @@
         <v>420</v>
       </c>
       <c r="G9">
-        <f>F9*D9</f>
+        <f t="shared" si="1"/>
         <v>420</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>462.00000000000006</v>
       </c>
       <c r="I9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="C10">
         <v>505</v>
@@ -2763,23 +2889,26 @@
         <v>419</v>
       </c>
       <c r="G10">
-        <f>F10*D10</f>
+        <f t="shared" si="1"/>
         <v>419</v>
       </c>
       <c r="H10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>460.90000000000003</v>
       </c>
       <c r="I10" t="s">
-        <v>42</v>
+        <v>68</v>
+      </c>
+      <c r="J10" t="s">
+        <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C11">
         <v>11</v>
@@ -2795,18 +2924,21 @@
         <v>35</v>
       </c>
       <c r="G11">
-        <f>F11*D11</f>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38.5</v>
       </c>
       <c r="I11" t="s">
-        <v>58</v>
+        <v>62</v>
+      </c>
+      <c r="J11" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -2827,18 +2959,21 @@
         <v>20</v>
       </c>
       <c r="G12">
-        <f>F12*D12</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="H12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="I12" t="s">
-        <v>57</v>
+        <v>71</v>
+      </c>
+      <c r="J12" t="s">
+        <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -2859,18 +2994,21 @@
         <v>300</v>
       </c>
       <c r="G13">
-        <f>F13*D13</f>
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
       <c r="H13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>330</v>
       </c>
       <c r="I13" t="s">
-        <v>60</v>
+        <v>72</v>
+      </c>
+      <c r="J13" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -2884,25 +3022,28 @@
         <v>10</v>
       </c>
       <c r="E14">
-        <f>D14*C14/2</f>
-        <v>165</v>
+        <f>D14*C14</f>
+        <v>330</v>
       </c>
       <c r="F14">
         <v>10</v>
       </c>
       <c r="G14">
-        <f>F14*D14</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="H14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>110.00000000000001</v>
       </c>
       <c r="I14" t="s">
-        <v>46</v>
+        <v>73</v>
+      </c>
+      <c r="J14" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -2923,23 +3064,26 @@
         <v>50</v>
       </c>
       <c r="G15">
-        <f>F15*D15</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="H15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>55.000000000000007</v>
       </c>
       <c r="I15" t="s">
-        <v>47</v>
+        <v>62</v>
+      </c>
+      <c r="J15" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C16">
         <v>100</v>
@@ -2955,20 +3099,23 @@
         <v>100</v>
       </c>
       <c r="G16">
-        <f>F16*D16</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="H16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>110.00000000000001</v>
       </c>
+      <c r="I16" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C17">
         <v>500</v>
@@ -2984,18 +3131,21 @@
         <v>200</v>
       </c>
       <c r="G17">
-        <f>F17*D17</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="H17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>220.00000000000003</v>
       </c>
       <c r="I17" t="s">
-        <v>62</v>
+        <v>74</v>
+      </c>
+      <c r="J17" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -3016,21 +3166,24 @@
         <v>100</v>
       </c>
       <c r="G18">
-        <f>F18*D18</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="H18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>110.00000000000001</v>
       </c>
+      <c r="I18" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>29</v>
       </c>
       <c r="E19">
         <f>SUM(E2:E18)</f>
-        <v>2927</v>
+        <v>3092</v>
       </c>
       <c r="G19">
         <f>SUM(G2:G18)</f>
@@ -3040,27 +3193,27 @@
         <f>SUM(H2:H18)</f>
         <v>6565.9</v>
       </c>
-      <c r="I19" t="s">
-        <v>61</v>
+      <c r="J19" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E20">
         <f>E19*1.2</f>
-        <v>3512.4</v>
+        <v>3710.3999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E29">
         <f>E2+E3+E4</f>
@@ -3071,9 +3224,9 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E30">
         <f>E10</f>
@@ -3084,22 +3237,22 @@
         <v>419</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E31">
         <f>E13+E14+E17</f>
-        <v>1065</v>
+        <v>1230</v>
       </c>
       <c r="G31">
         <f>G13+G14+G17</f>
         <v>600</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E32">
         <f>E5+E6+E7+E8+E9+E11+E12</f>
@@ -3112,7 +3265,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E33">
         <f>E18+E16+E15</f>
@@ -3126,7 +3279,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{E3AECD96-9123-4BF5-A94E-CE5B0E97959C}"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{E3AECD96-9123-4BF5-A94E-CE5B0E97959C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>